<commit_message>
end of day 4 sprint backlog update
</commit_message>
<xml_diff>
--- a/Sprint 1 Documentation/SprintBacklog.xlsx
+++ b/Sprint 1 Documentation/SprintBacklog.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_6f\AC\Temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_6dd\AC\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8BF322CD-2D02-41D9-9553-610B026E04BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BA26BF87-E9E5-48BF-B477-F972977A9FDB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="76">
   <si>
     <t>Backlog Task &amp; ID</t>
   </si>
@@ -121,115 +121,118 @@
     <t>Add validation for input</t>
   </si>
   <si>
+    <t>AG, AI</t>
+  </si>
+  <si>
+    <t>2. As a customer, I can search based on procedure</t>
+  </si>
+  <si>
+    <t>3. As a customer, I can search based on location</t>
+  </si>
+  <si>
+    <t>Create multiple search bars on webpage allowing user input</t>
+  </si>
+  <si>
+    <t>Access the device's co-ordinates to enable a LIVE Location search</t>
+  </si>
+  <si>
+    <t>WM, AI, AR</t>
+  </si>
+  <si>
+    <t>28/1/2020</t>
+  </si>
+  <si>
+    <t>Assign co-ordinates to all providers in the database</t>
+  </si>
+  <si>
+    <t>AR</t>
+  </si>
+  <si>
+    <t>8. As a customer, I can view search results in a list</t>
+  </si>
+  <si>
+    <t>Create results page for website to return list</t>
+  </si>
+  <si>
+    <t>Return list from database</t>
+  </si>
+  <si>
+    <t>9. As a customer, I can view search results on a map</t>
+  </si>
+  <si>
+    <t>Research map API functionality</t>
+  </si>
+  <si>
+    <t>AR, WM,AI</t>
+  </si>
+  <si>
+    <t>AI,WM</t>
+  </si>
+  <si>
+    <t>Return results from database, nearest to location</t>
+  </si>
+  <si>
+    <t>12. As a customer, I can view details of a search result in the list</t>
+  </si>
+  <si>
+    <t>Access a further details page on a specific search result (button call)</t>
+  </si>
+  <si>
+    <t>Not Started</t>
+  </si>
+  <si>
+    <t>Return full set of details on a specific provider ID from DB</t>
+  </si>
+  <si>
+    <t>4. As a customer, I can sort search results based on price</t>
+  </si>
+  <si>
+    <t>Sort by button option on UI (API call)</t>
+  </si>
+  <si>
+    <t>Return list from database in order of price</t>
+  </si>
+  <si>
+    <t>6. As a customer, I can sort search results based on location</t>
+  </si>
+  <si>
+    <t>Sort by location button on UI (API call)</t>
+  </si>
+  <si>
+    <t>Return list from database in order of distance from address</t>
+  </si>
+  <si>
+    <t>13. As a customer, I can view details of a search result on a map</t>
+  </si>
+  <si>
+    <t>10. As a customer, I can set a price range for my search</t>
+  </si>
+  <si>
+    <t>Price range option on UI</t>
+  </si>
+  <si>
+    <t>AI, AG</t>
+  </si>
+  <si>
+    <t>Return list from database between a price range</t>
+  </si>
+  <si>
+    <t>11. As a customer, I can set a distance range for my search</t>
+  </si>
+  <si>
+    <t>Distance range option on UI</t>
+  </si>
+  <si>
+    <t>Return list from database between a distance range</t>
+  </si>
+  <si>
+    <t>16. As a customer, I can view service provider information page</t>
+  </si>
+  <si>
+    <t>Design CraneWare contact page</t>
+  </si>
+  <si>
     <t>AG</t>
-  </si>
-  <si>
-    <t>2. As a customer, I can search based on procedure</t>
-  </si>
-  <si>
-    <t>3. As a customer, I can search based on location</t>
-  </si>
-  <si>
-    <t>Create multiple search bars on webpage allowing user input</t>
-  </si>
-  <si>
-    <t>AG, AI</t>
-  </si>
-  <si>
-    <t>Access the device's co-ordinates to enable a LIVE Location search</t>
-  </si>
-  <si>
-    <t>WM, AI, AR</t>
-  </si>
-  <si>
-    <t>28/1/2020</t>
-  </si>
-  <si>
-    <t>Assign co-ordinates to all providers in the database</t>
-  </si>
-  <si>
-    <t>AR</t>
-  </si>
-  <si>
-    <t>8. As a customer, I can view search results in a list</t>
-  </si>
-  <si>
-    <t>Create results page for website to return list</t>
-  </si>
-  <si>
-    <t>Return list from database</t>
-  </si>
-  <si>
-    <t>9. As a customer, I can view search results on a map</t>
-  </si>
-  <si>
-    <t>Research map API functionality</t>
-  </si>
-  <si>
-    <t>AR, WM,AI</t>
-  </si>
-  <si>
-    <t>Return results from database, nearest to location</t>
-  </si>
-  <si>
-    <t>12. As a customer, I can view details of a search result in the list</t>
-  </si>
-  <si>
-    <t>Access a further details page on a specific search result (button call)</t>
-  </si>
-  <si>
-    <t>Not Started</t>
-  </si>
-  <si>
-    <t>Return full set of details on a specific provider ID from DB</t>
-  </si>
-  <si>
-    <t>4. As a customer, I can sort search results based on price</t>
-  </si>
-  <si>
-    <t>Sort by button option on UI (API call)</t>
-  </si>
-  <si>
-    <t>Return list from database in order of price</t>
-  </si>
-  <si>
-    <t>6. As a customer, I can sort search results based on location</t>
-  </si>
-  <si>
-    <t>Sort by location button on UI (API call)</t>
-  </si>
-  <si>
-    <t>Return list from database in order of distance from address</t>
-  </si>
-  <si>
-    <t>13. As a customer, I can view details of a search result on a map</t>
-  </si>
-  <si>
-    <t>10. As a customer, I can set a price range for my search</t>
-  </si>
-  <si>
-    <t>Price range option on UI</t>
-  </si>
-  <si>
-    <t>AI, AG</t>
-  </si>
-  <si>
-    <t>Return list from database between a price range</t>
-  </si>
-  <si>
-    <t>11. As a customer, I can set a distance range for my search</t>
-  </si>
-  <si>
-    <t>Distance range option on UI</t>
-  </si>
-  <si>
-    <t>Return list from database between a distance range</t>
-  </si>
-  <si>
-    <t>16. As a customer, I can view service provider information page</t>
-  </si>
-  <si>
-    <t>Design CraneWare contact page</t>
   </si>
   <si>
     <t>7. As a customer, I can sort search results based on "best match"</t>
@@ -672,8 +675,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="I63" sqref="I63"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="J67" sqref="J67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -758,6 +761,9 @@
       <c r="H3">
         <v>0</v>
       </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:12">
       <c r="A4" t="s">
@@ -781,6 +787,9 @@
       <c r="H4">
         <v>0</v>
       </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:12" s="1" customFormat="1">
       <c r="A5" s="1" t="s">
@@ -813,6 +822,9 @@
       <c r="H6" s="5">
         <v>0</v>
       </c>
+      <c r="I6" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:12">
       <c r="A7" t="s">
@@ -836,6 +848,9 @@
       <c r="H7">
         <v>2</v>
       </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:12">
       <c r="A8" t="s">
@@ -859,6 +874,9 @@
       <c r="H8">
         <v>0</v>
       </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" t="s">
@@ -882,6 +900,9 @@
       <c r="H9">
         <v>2</v>
       </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
       <c r="L9" t="s">
         <v>27</v>
       </c>
@@ -894,7 +915,7 @@
         <v>29</v>
       </c>
       <c r="D10" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E10">
         <v>2</v>
@@ -907,6 +928,9 @@
       </c>
       <c r="H10">
         <v>1</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
       </c>
       <c r="L10" t="s">
         <v>27</v>
@@ -943,6 +967,9 @@
       <c r="H12" s="5">
         <v>0</v>
       </c>
+      <c r="I12" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:12" s="5" customFormat="1">
       <c r="A13" t="s">
@@ -967,6 +994,9 @@
       <c r="H13" s="5">
         <v>2</v>
       </c>
+      <c r="I13" s="5">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" spans="1:12">
       <c r="A14" t="s">
@@ -990,6 +1020,9 @@
       <c r="H14">
         <v>0</v>
       </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:12">
       <c r="A15" t="s">
@@ -1013,6 +1046,9 @@
       <c r="H15">
         <v>2</v>
       </c>
+      <c r="I15">
+        <v>1</v>
+      </c>
       <c r="L15" t="s">
         <v>27</v>
       </c>
@@ -1030,10 +1066,10 @@
         <v>32</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E17" s="5">
         <v>2</v>
@@ -1046,14 +1082,17 @@
       </c>
       <c r="H17" s="5">
         <v>1</v>
+      </c>
+      <c r="I17" s="5">
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:12" s="5" customFormat="1">
       <c r="A18" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" s="5" t="s">
         <v>34</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>35</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>16</v>
@@ -1070,8 +1109,11 @@
       <c r="H18" s="5">
         <v>0</v>
       </c>
+      <c r="I18" s="5">
+        <v>0</v>
+      </c>
       <c r="L18" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:12" s="5" customFormat="1">
@@ -1096,13 +1138,16 @@
       <c r="H19" s="5">
         <v>2</v>
       </c>
+      <c r="I19" s="5">
+        <v>1</v>
+      </c>
     </row>
     <row r="20" spans="1:12" s="5" customFormat="1">
       <c r="A20" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" s="5" t="s">
         <v>37</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>38</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>16</v>
@@ -1117,6 +1162,9 @@
         <v>3</v>
       </c>
       <c r="H20" s="5">
+        <v>0</v>
+      </c>
+      <c r="I20" s="5">
         <v>0</v>
       </c>
     </row>
@@ -1142,6 +1190,9 @@
       <c r="H21">
         <v>0</v>
       </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
     </row>
     <row r="22" spans="1:12">
       <c r="A22" t="s">
@@ -1165,13 +1216,16 @@
       <c r="H22">
         <v>3</v>
       </c>
+      <c r="I22">
+        <v>1</v>
+      </c>
       <c r="L22" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:12" s="1" customFormat="1">
       <c r="A23" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B23" s="1">
         <v>8</v>
@@ -1179,10 +1233,10 @@
     </row>
     <row r="24" spans="1:12">
       <c r="A24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C24" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D24" t="s">
         <v>22</v>
@@ -1198,6 +1252,9 @@
       </c>
       <c r="H24">
         <v>2</v>
+      </c>
+      <c r="I24">
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:12">
@@ -1222,10 +1279,13 @@
       <c r="H25">
         <v>2</v>
       </c>
+      <c r="I25">
+        <v>1</v>
+      </c>
     </row>
     <row r="26" spans="1:12">
       <c r="A26" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C26" t="s">
         <v>24</v>
@@ -1243,6 +1303,9 @@
         <v>0</v>
       </c>
       <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26">
         <v>0</v>
       </c>
     </row>
@@ -1268,13 +1331,16 @@
       <c r="H27">
         <v>0.5</v>
       </c>
+      <c r="I27">
+        <v>0</v>
+      </c>
       <c r="L27" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="28" spans="1:12" s="1" customFormat="1">
       <c r="A28" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B28" s="1">
         <v>8</v>
@@ -1282,10 +1348,10 @@
     </row>
     <row r="29" spans="1:12">
       <c r="A29" t="s">
+        <v>42</v>
+      </c>
+      <c r="C29" t="s">
         <v>43</v>
-      </c>
-      <c r="C29" t="s">
-        <v>44</v>
       </c>
       <c r="D29" t="s">
         <v>16</v>
@@ -1300,6 +1366,9 @@
         <v>0</v>
       </c>
       <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="I29">
         <v>0</v>
       </c>
     </row>
@@ -1308,7 +1377,7 @@
         <v>20</v>
       </c>
       <c r="C30" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="D30" t="s">
         <v>22</v>
@@ -1324,6 +1393,9 @@
       </c>
       <c r="H30">
         <v>2</v>
+      </c>
+      <c r="I30">
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:12">
@@ -1348,6 +1420,9 @@
       <c r="H31">
         <v>0</v>
       </c>
+      <c r="I31">
+        <v>0</v>
+      </c>
     </row>
     <row r="32" spans="1:12">
       <c r="A32" t="s">
@@ -1371,6 +1446,9 @@
       <c r="H32">
         <v>0.5</v>
       </c>
+      <c r="I32">
+        <v>0</v>
+      </c>
       <c r="L32" t="s">
         <v>27</v>
       </c>
@@ -1402,6 +1480,9 @@
       <c r="H34">
         <v>2</v>
       </c>
+      <c r="I34">
+        <v>2</v>
+      </c>
     </row>
     <row r="35" spans="1:12">
       <c r="A35" t="s">
@@ -1425,6 +1506,9 @@
       <c r="H35">
         <v>0</v>
       </c>
+      <c r="I35">
+        <v>0</v>
+      </c>
     </row>
     <row r="36" spans="1:12" s="1" customFormat="1">
       <c r="A36" s="1" t="s">
@@ -1439,7 +1523,7 @@
         <v>51</v>
       </c>
       <c r="C37" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="D37" t="s">
         <v>22</v>
@@ -1454,6 +1538,9 @@
         <v>2</v>
       </c>
       <c r="H37">
+        <v>2</v>
+      </c>
+      <c r="I37">
         <v>2</v>
       </c>
     </row>
@@ -1479,6 +1566,9 @@
       <c r="H38">
         <v>2</v>
       </c>
+      <c r="I38">
+        <v>2</v>
+      </c>
     </row>
     <row r="39" spans="1:12">
       <c r="A39" t="s">
@@ -1502,6 +1592,9 @@
       <c r="H39">
         <v>1</v>
       </c>
+      <c r="I39">
+        <v>1</v>
+      </c>
       <c r="L39" t="s">
         <v>27</v>
       </c>
@@ -1519,7 +1612,7 @@
         <v>54</v>
       </c>
       <c r="C41" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="D41" t="s">
         <v>22</v>
@@ -1534,6 +1627,9 @@
         <v>2</v>
       </c>
       <c r="H41">
+        <v>2</v>
+      </c>
+      <c r="I41">
         <v>2</v>
       </c>
     </row>
@@ -1545,7 +1641,7 @@
         <v>24</v>
       </c>
       <c r="D42" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E42">
         <v>2</v>
@@ -1557,6 +1653,9 @@
         <v>2</v>
       </c>
       <c r="H42">
+        <v>0</v>
+      </c>
+      <c r="I42">
         <v>0</v>
       </c>
     </row>
@@ -1582,6 +1681,9 @@
       <c r="H43">
         <v>1</v>
       </c>
+      <c r="I43">
+        <v>1</v>
+      </c>
       <c r="L43" t="s">
         <v>27</v>
       </c>
@@ -1613,6 +1715,9 @@
       <c r="H45">
         <v>2</v>
       </c>
+      <c r="I45">
+        <v>2</v>
+      </c>
     </row>
     <row r="46" spans="1:12">
       <c r="A46" t="s">
@@ -1622,7 +1727,7 @@
         <v>24</v>
       </c>
       <c r="D46" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E46">
         <v>1</v>
@@ -1634,6 +1739,9 @@
         <v>1</v>
       </c>
       <c r="H46">
+        <v>0</v>
+      </c>
+      <c r="I46">
         <v>0</v>
       </c>
     </row>
@@ -1667,11 +1775,17 @@
       <c r="H48">
         <v>0</v>
       </c>
+      <c r="I48">
+        <v>0</v>
+      </c>
     </row>
     <row r="49" spans="1:12">
       <c r="A49" t="s">
         <v>20</v>
       </c>
+      <c r="C49" t="s">
+        <v>59</v>
+      </c>
       <c r="D49" s="3" t="s">
         <v>48</v>
       </c>
@@ -1685,6 +1799,9 @@
         <v>2</v>
       </c>
       <c r="H49">
+        <v>2</v>
+      </c>
+      <c r="I49">
         <v>2</v>
       </c>
     </row>
@@ -1710,6 +1827,9 @@
       <c r="H50">
         <v>0</v>
       </c>
+      <c r="I50">
+        <v>0</v>
+      </c>
     </row>
     <row r="51" spans="1:12">
       <c r="A51" t="s">
@@ -1767,11 +1887,17 @@
       <c r="H53">
         <v>0</v>
       </c>
+      <c r="I53">
+        <v>0</v>
+      </c>
     </row>
     <row r="54" spans="1:12">
       <c r="A54" t="s">
         <v>20</v>
       </c>
+      <c r="C54" t="s">
+        <v>59</v>
+      </c>
       <c r="D54" s="3" t="s">
         <v>48</v>
       </c>
@@ -1785,6 +1911,9 @@
         <v>2</v>
       </c>
       <c r="H54">
+        <v>2</v>
+      </c>
+      <c r="I54">
         <v>2</v>
       </c>
     </row>
@@ -1810,6 +1939,9 @@
       <c r="H55">
         <v>0</v>
       </c>
+      <c r="I55">
+        <v>2</v>
+      </c>
     </row>
     <row r="56" spans="1:12">
       <c r="A56" t="s">
@@ -1833,6 +1965,9 @@
       <c r="H56">
         <v>2</v>
       </c>
+      <c r="I56">
+        <v>2</v>
+      </c>
       <c r="L56" t="s">
         <v>27</v>
       </c>
@@ -1850,7 +1985,7 @@
         <v>65</v>
       </c>
       <c r="C58" t="s">
-        <v>29</v>
+        <v>66</v>
       </c>
       <c r="D58" t="s">
         <v>16</v>
@@ -1865,6 +2000,9 @@
         <v>0</v>
       </c>
       <c r="H58">
+        <v>0</v>
+      </c>
+      <c r="I58">
         <v>0</v>
       </c>
     </row>
@@ -1873,7 +2011,7 @@
         <v>17</v>
       </c>
       <c r="C59" t="s">
-        <v>29</v>
+        <v>66</v>
       </c>
       <c r="D59" t="s">
         <v>22</v>
@@ -1890,10 +2028,13 @@
       <c r="H59">
         <v>1</v>
       </c>
+      <c r="I59">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="60" spans="1:12" s="1" customFormat="1">
       <c r="A60" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B60" s="1">
         <v>2</v>
@@ -1901,7 +2042,7 @@
     </row>
     <row r="61" spans="1:12">
       <c r="A61" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C61" t="s">
         <v>59</v>
@@ -1921,13 +2062,16 @@
       <c r="H61">
         <v>0</v>
       </c>
+      <c r="I61">
+        <v>0</v>
+      </c>
     </row>
     <row r="62" spans="1:12">
       <c r="A62" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C62" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D62" t="s">
         <v>22</v>
@@ -1944,10 +2088,13 @@
       <c r="H62">
         <v>0.5</v>
       </c>
+      <c r="I62">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="63" spans="1:12">
       <c r="A63" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D63" t="s">
         <v>48</v>
@@ -1962,6 +2109,9 @@
         <v>2</v>
       </c>
       <c r="H63">
+        <v>2</v>
+      </c>
+      <c r="I63">
         <v>2</v>
       </c>
     </row>
@@ -1987,13 +2137,16 @@
       <c r="H64">
         <v>2</v>
       </c>
+      <c r="I64">
+        <v>2</v>
+      </c>
       <c r="L64" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="65" spans="1:10" s="9" customFormat="1">
       <c r="A65" s="9" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E65" s="9">
         <f t="shared" ref="E65:J65" si="0">SUM(E3:E63)</f>
@@ -2013,7 +2166,7 @@
       </c>
       <c r="I65" s="9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="J65" s="9">
         <f t="shared" si="0"/>
@@ -2086,10 +2239,10 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
@@ -2121,7 +2274,7 @@
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -2136,7 +2289,7 @@
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -2154,7 +2307,7 @@
     </row>
     <row r="9" spans="1:11">
       <c r="A9" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -2169,7 +2322,7 @@
     </row>
     <row r="11" spans="1:11">
       <c r="A11" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -2184,7 +2337,7 @@
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -2199,7 +2352,7 @@
     </row>
     <row r="16" spans="1:11">
       <c r="A16" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>

</xml_diff>